<commit_message>
Actualizacion del archivo de riesgos
</commit_message>
<xml_diff>
--- a/Seguimiento/Soporte-riesgos/SeguimientoActualizaciónTiemposGithub.xlsx
+++ b/Seguimiento/Soporte-riesgos/SeguimientoActualizaciónTiemposGithub.xlsx
@@ -89,7 +89,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-septiembre 15 - septiembre 21</t>
+septiembre 15 - septiembre 21 Semana de trabajo individual
+</t>
         </r>
       </text>
     </comment>
@@ -282,6 +283,54 @@
           </rPr>
           <t xml:space="preserve">
 noviembre 10-noviembre 16</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+noviembre 17-noviembre 27</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No tenia asignadas tareas para esta semana</t>
         </r>
       </text>
     </comment>
@@ -290,7 +339,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
   <si>
     <t>Ciclo2 Semana 1</t>
   </si>
@@ -344,13 +393,19 @@
   </si>
   <si>
     <t>Ciclo 3 Semana 6</t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,6 +433,19 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -393,7 +461,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -402,16 +470,178 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -419,27 +649,47 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -741,10 +991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,71 +1002,192 @@
     <col min="8" max="8" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="39" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:13" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="15" t="s">
         <v>11</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="16" t="s">
         <v>12</v>
       </c>
+      <c r="B3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="6"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="16" t="s">
         <v>13</v>
       </c>
+      <c r="B4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="6"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="16" t="s">
         <v>14</v>
       </c>
+      <c r="B5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="6"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="16" t="s">
         <v>15</v>
       </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="6"/>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>